<commit_message>
RH-7067 RP referral, Import, edit patient consent change
</commit_message>
<xml_diff>
--- a/force-app/main/default/staticresources/Import_Patient_Template.xlsx
+++ b/force-app/main/default/staticresources/Import_Patient_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q1057161\Desktop\RP Revamp\Dec Release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u1119317\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9EDCE6-2670-4D78-83EC-395156F23E48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEBC6F9-D100-43D0-9F13-CA6E099F06AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EA544E7C-104C-4CC4-B22E-BDDCF0D09CF8}"/>
   </bookViews>
@@ -134,29 +134,6 @@
     <t>Patient Alternative Phone</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"My patient, and/or patient's legal guardian if applicable, agrees to share their contact information and patient's pre-screener data with IQVIA and its affiliates, and the study doctors, so that they may contact the patient and/or their delegate regarding study participation."</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  Options: Yes/No  To indicate whether the RP has the authorization from the patient or  blank when not filled. Required Only if the file has Personal Information</t>
-    </r>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -221,6 +198,29 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">  Mandatory for a minor participant.  Enter Yes to attest the delegate is of/over the age of legal majority</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"My patient, and/or patient's legal guardian if applicable, agrees to share their information with a study team, and to be contacted at the telephone number(s) and email they have provided, and via automated dialing, and/or artificial or pre-recorded voice, to schedule study appointments and keep them updated with important study-related information.  Their consent is not required as a condition of purchasing any property, goods, or services."</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  Options: Yes/No. To indicate whether the RP has the authorization from the patient or blank when not filled. Required Only if the file has Personal Information</t>
     </r>
   </si>
 </sst>
@@ -615,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4874A4A3-0CD4-4513-BA5F-71E99146205B}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -626,7 +626,8 @@
     <col min="3" max="3" width="20.7265625" style="5" customWidth="1"/>
     <col min="4" max="4" width="14.6328125" style="5" customWidth="1"/>
     <col min="5" max="5" width="13.08984375" style="5" customWidth="1"/>
-    <col min="6" max="9" width="8.7265625" style="5"/>
+    <col min="6" max="8" width="8.7265625" style="5"/>
+    <col min="9" max="9" width="15.81640625" style="5" customWidth="1"/>
     <col min="10" max="10" width="18.1796875" style="5" customWidth="1"/>
     <col min="11" max="11" width="16.453125" style="5" customWidth="1"/>
     <col min="12" max="12" width="17.90625" style="5" customWidth="1"/>
@@ -645,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -663,7 +664,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>6</v>
@@ -672,7 +673,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>8</v>
@@ -731,19 +732,19 @@
         <v>22</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>23</v>
@@ -761,7 +762,7 @@
         <v>26</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>27</v>
@@ -773,7 +774,7 @@
         <v>29</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>